<commit_message>
Added ADS1115 to parts
Missed part, change R8 to zero ohms
</commit_message>
<xml_diff>
--- a/AutoSteerPCB/PartsList.xlsx
+++ b/AutoSteerPCB/PartsList.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="161">
   <si>
     <t>Manufacturer Part Number</t>
   </si>
@@ -482,6 +482,21 @@
   </si>
   <si>
     <t>Arduino (EBAY, Amazon)</t>
+  </si>
+  <si>
+    <t>ADS1115 - 16 bit A/D convertor</t>
+  </si>
+  <si>
+    <t>AdaFruit, Ebay, Amazon</t>
+  </si>
+  <si>
+    <t>16 bit A/D convertor on BO board</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/1085</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/13926</t>
   </si>
 </sst>
 </file>
@@ -535,7 +550,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -554,6 +569,10 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -855,7 +874,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B36" sqref="B36"/>
+      <selection pane="bottomRight" activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1638,36 +1657,38 @@
     <row r="33" spans="1:8">
       <c r="F33" s="6"/>
       <c r="G33" s="6"/>
+      <c r="H33" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="C34" s="4" t="s">
+      <c r="A34" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="C34" s="9" t="s">
         <v>126</v>
       </c>
       <c r="E34" s="2">
         <v>1</v>
       </c>
-      <c r="F34" s="6">
+      <c r="F34" s="7">
         <v>12</v>
       </c>
-      <c r="G34" s="6">
+      <c r="G34" s="7">
         <v>12</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>142</v>
+        <v>158</v>
       </c>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="3"/>
-      <c r="F35" s="6"/>
-      <c r="G35" s="6"/>
+      <c r="A35" s="8"/>
+      <c r="B35" s="9"/>
       <c r="H35" t="s">
-        <v>143</v>
+        <v>159</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -1792,12 +1813,35 @@
       </c>
     </row>
     <row r="44" spans="1:8">
-      <c r="F44" s="6"/>
-      <c r="G44" s="6"/>
+      <c r="A44" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="E44" s="2">
+        <v>1</v>
+      </c>
+      <c r="F44" s="6">
+        <v>12</v>
+      </c>
+      <c r="G44" s="6">
+        <v>12</v>
+      </c>
+      <c r="H44" s="4" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="45" spans="1:8">
+      <c r="A45" s="3"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
+      <c r="H45" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="46" spans="1:8">
       <c r="F46" s="6"/>

</xml_diff>